<commit_message>
Small rename in the case title value
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -363,7 +363,7 @@
     <t>timesheet</t>
   </si>
   <si>
-    <t>Review/Approve</t>
+    <t>Review and Approve</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1551,7 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added buckslip complaint rule
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,158 +26,158 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">ruleName</t>
+          <t>ruleName</t>
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">fileType</t>
+          <t>fileType</t>
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0">
+    <comment ref="D16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">startProcess</t>
+          <t>startProcess</t>
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0">
+    <comment ref="E16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">processName</t>
+          <t>processName</t>
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0">
+    <comment ref="F16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">priority</t>
+          <t>priority</t>
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0">
+    <comment ref="G16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0">
+    <comment ref="H16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0">
+    <comment ref="I16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0">
+    <comment ref="J16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0">
+    <comment ref="K16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
@@ -182,39 +186,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
-  <si>
-    <t xml:space="preserve">RuleSet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form Workflow Rules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.EvaluationContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.ExpressionParser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.spel.standard.SpelExpressionParser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.spel.support.StandardEvaluationContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.armedia.acm.plugins.ecm.workflow.EcmFileWorkflowConfiguration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">function Boolean evalSpring(String expression, Object obj)
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+  <si>
+    <t>RuleSet</t>
+  </si>
+  <si>
+    <t>Form Workflow Rules</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.EvaluationContext</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.Expression</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.ExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.standard.SpelExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.support.StandardEvaluationContext</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.plugins.ecm.workflow.EcmFileWorkflowConfiguration</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>function Boolean evalSpring(String expression, Object obj)
 {
     ExpressionParser ep = new SpelExpressionParser();
     Expression exp = ep.parseExpression(expression);
@@ -224,180 +228,164 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Sequential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RuleTable Form Workflow Rules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONDITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file: EcmFileWorkflowConfiguration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ecmFile.fileType.equalsIgnoreCase("$param") || "$param".equals("*")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setStartProcess($param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setProcessName("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setTaskPriority($param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setTaskDueDateExpression("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setTaskName("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setApprovers("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setRequestType("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setBuckslipProcess($param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If different rules apply to the same document, the last rule wins.  Be sure to put default rules first, and specific rules later.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start a Workflow Process? (true/false)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of business process to start (must be an Activiti process name)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority of user tasks (must be a number between 0 and 100; higher number is higher priority)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due date of user tasks.  Must be a valid ISO801 duration expression.  Examples: P3D = three days from now; P3H = 3 hours from now.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma-separated list of user ids; these users will be the reviewers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Business-meaningful process name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is buckslip process?               false is by default.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Workflow (no other rules match)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close Complaint Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">close_complaint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acmDocumentWorkflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report of Investigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buckslip Complaint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complaint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ArkCaseBuckslipProcess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ann-acm@armedia.com,ian-acm@armedia.com,samuel-acm@armedia.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Case Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">change_case_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buckslip Case File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review and Approve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Costsheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costsheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timesheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timesheet</t>
+    <t>Sequential</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>RuleTable Form Workflow Rules</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>$file: EcmFileWorkflowConfiguration</t>
+  </si>
+  <si>
+    <t>ecmFile.fileType.equalsIgnoreCase("$param") || "$param".equals("*")</t>
+  </si>
+  <si>
+    <t>$file.setStartProcess($param);</t>
+  </si>
+  <si>
+    <t>$file.setProcessName("$param");</t>
+  </si>
+  <si>
+    <t>$file.setTaskPriority($param);</t>
+  </si>
+  <si>
+    <t>$file.setTaskDueDateExpression("$param");</t>
+  </si>
+  <si>
+    <t>$file.setTaskName("$param");</t>
+  </si>
+  <si>
+    <t>$file.setApprovers("$param");</t>
+  </si>
+  <si>
+    <t>$file.setRequestType("$param");</t>
+  </si>
+  <si>
+    <t>$file.setBuckslipProcess($param);</t>
+  </si>
+  <si>
+    <t>If different rules apply to the same document, the last rule wins.  Be sure to put default rules first, and specific rules later.</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>File Type</t>
+  </si>
+  <si>
+    <t>Start a Workflow Process? (true/false)</t>
+  </si>
+  <si>
+    <t>Name of business process to start (must be an Activiti process name)</t>
+  </si>
+  <si>
+    <t>Priority of user tasks (must be a number between 0 and 100; higher number is higher priority)</t>
+  </si>
+  <si>
+    <t>Due date of user tasks.  Must be a valid ISO801 duration expression.  Examples: P3D = three days from now; P3H = 3 hours from now.</t>
+  </si>
+  <si>
+    <t>Task name</t>
+  </si>
+  <si>
+    <t>Comma-separated list of user ids; these users will be the reviewers.</t>
+  </si>
+  <si>
+    <t>Business-meaningful process name</t>
+  </si>
+  <si>
+    <t>is buckslip process?               false is by default.</t>
+  </si>
+  <si>
+    <t>Default Workflow (no other rules match)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Close Complaint Request</t>
+  </si>
+  <si>
+    <t>close_complaint</t>
+  </si>
+  <si>
+    <t>acmDocumentWorkflow</t>
+  </si>
+  <si>
+    <t>P3D</t>
+  </si>
+  <si>
+    <t>Report of Investigation</t>
+  </si>
+  <si>
+    <t>roi</t>
+  </si>
+  <si>
+    <t>Buckslip Complaint</t>
+  </si>
+  <si>
+    <t>complaint</t>
+  </si>
+  <si>
+    <t>ArkCaseBuckslipProcess</t>
+  </si>
+  <si>
+    <t>ann-acm@armedia.com,ian-acm@armedia.com,samuel-acm@armedia.com</t>
+  </si>
+  <si>
+    <t>Change Case Status</t>
+  </si>
+  <si>
+    <t>change_case_status</t>
+  </si>
+  <si>
+    <t>Buckslip Case File</t>
+  </si>
+  <si>
+    <t>case_file</t>
+  </si>
+  <si>
+    <t>Review and Approve</t>
+  </si>
+  <si>
+    <t>Costsheet</t>
+  </si>
+  <si>
+    <t>costsheet</t>
+  </si>
+  <si>
+    <t>Timesheet</t>
+  </si>
+  <si>
+    <t>timesheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -407,7 +395,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -466,230 +454,230 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -748,13 +736,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -768,9 +772,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -782,7 +792,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -792,9 +802,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -813,9 +829,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -827,7 +849,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -837,9 +859,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -858,9 +886,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -872,7 +906,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -882,9 +916,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -903,9 +943,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -917,7 +963,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -927,9 +973,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -948,9 +1000,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -962,7 +1020,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -972,9 +1030,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -993,9 +1057,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1007,7 +1077,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1017,9 +1087,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1038,9 +1114,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1052,7 +1134,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1062,9 +1144,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1083,9 +1171,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="9" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1097,7 +1191,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1107,9 +1201,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1128,9 +1228,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="10" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1142,7 +1248,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1152,9 +1258,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1173,9 +1285,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="11" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1187,7 +1305,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1197,46 +1315,836 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1044" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1042" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1040" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1038" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1036" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1034" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="65.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.71"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="65.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1245,7 +2153,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -1258,7 +2166,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -1271,7 +2179,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
@@ -1284,7 +2192,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="s">
@@ -1297,7 +2205,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5" t="s">
@@ -1310,7 +2218,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
@@ -1323,7 +2231,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7" t="s">
@@ -1336,7 +2244,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
@@ -1349,7 +2257,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10" t="s">
@@ -1362,7 +2270,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1371,7 +2279,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
@@ -1386,7 +2294,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="7" t="s">
@@ -1417,7 +2325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="7" t="s">
@@ -1432,7 +2340,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="13" t="s">
@@ -1463,7 +2371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>26</v>
       </c>
@@ -1498,7 +2406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>37</v>
@@ -1517,7 +2425,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="20" t="s">
         <v>40</v>
@@ -1531,7 +2439,7 @@
       <c r="E18" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="23" t="n">
+      <c r="F18" s="23">
         <v>50</v>
       </c>
       <c r="G18" s="23" t="s">
@@ -1542,7 +2450,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
         <v>44</v>
@@ -1556,7 +2464,7 @@
       <c r="E19" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="23" t="n">
+      <c r="F19" s="23">
         <v>50</v>
       </c>
       <c r="G19" s="23" t="s">
@@ -1567,7 +2475,7 @@
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="20" t="s">
         <v>46</v>
@@ -1581,13 +2489,15 @@
       <c r="E20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="23" t="n">
+      <c r="F20" s="23">
         <v>50</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="I20" s="23" t="s">
         <v>49</v>
       </c>
@@ -1596,7 +2506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>50</v>
@@ -1610,7 +2520,7 @@
       <c r="E21" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="23" t="n">
+      <c r="F21" s="23">
         <v>50</v>
       </c>
       <c r="G21" s="23" t="s">
@@ -1621,7 +2531,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="20" t="s">
         <v>52</v>
@@ -1635,7 +2545,7 @@
       <c r="E22" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="23" t="n">
+      <c r="F22" s="23">
         <v>50</v>
       </c>
       <c r="G22" s="23" t="s">
@@ -1652,7 +2562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
         <v>55</v>
@@ -1666,7 +2576,7 @@
       <c r="E23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="23" t="n">
+      <c r="F23" s="23">
         <v>50</v>
       </c>
       <c r="G23" s="23" t="s">
@@ -1677,7 +2587,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
         <v>57</v>
@@ -1691,7 +2601,7 @@
       <c r="E24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="23" t="n">
+      <c r="F24" s="23">
         <v>50</v>
       </c>
       <c r="G24" s="23" t="s">
@@ -1702,7 +2612,7 @@
       <c r="J24" s="23"/>
       <c r="K24" s="23"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="24"/>
@@ -1715,7 +2625,7 @@
       <c r="J25" s="23"/>
       <c r="K25" s="23"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
       <c r="C26" s="24"/>
@@ -1728,7 +2638,7 @@
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
       <c r="C27" s="24"/>
@@ -1741,7 +2651,7 @@
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="20"/>
       <c r="C28" s="24"/>
@@ -1756,70 +2666,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I22" r:id="rId2" display="ann-acm@armedia.com"/>
+    <hyperlink ref="I22" r:id="rId1" display="ann-acm@armedia.com"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.71"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.71"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AFDP-5540 New endpoint for getting groups by role
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,158 +26,158 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B16" authorId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">ruleName</t>
+          <t>ruleName</t>
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">fileType</t>
+          <t>fileType</t>
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0">
+    <comment ref="D16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">startProcess</t>
+          <t>startProcess</t>
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0">
+    <comment ref="E16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">processName</t>
+          <t>processName</t>
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0">
+    <comment ref="F16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">priority</t>
+          <t>priority</t>
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0">
+    <comment ref="G16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0">
+    <comment ref="H16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0">
+    <comment ref="I16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0">
+    <comment ref="J16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0">
+    <comment ref="K16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">dueDate</t>
+          <t>dueDate</t>
         </r>
       </text>
     </comment>
@@ -182,39 +186,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
-  <si>
-    <t xml:space="preserve">RuleSet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form Workflow Rules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.EvaluationContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.ExpressionParser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.spel.standard.SpelExpressionParser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.springframework.expression.spel.support.StandardEvaluationContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.armedia.acm.plugins.ecm.workflow.EcmFileWorkflowConfiguration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">function Boolean evalSpring(String expression, Object obj)
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+  <si>
+    <t>RuleSet</t>
+  </si>
+  <si>
+    <t>Form Workflow Rules</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.EvaluationContext</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.Expression</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.ExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.standard.SpelExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.support.StandardEvaluationContext</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.plugins.ecm.workflow.EcmFileWorkflowConfiguration</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>function Boolean evalSpring(String expression, Object obj)
 {
     ExpressionParser ep = new SpelExpressionParser();
     Expression exp = ep.parseExpression(expression);
@@ -224,180 +228,164 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Sequential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RuleTable Form Workflow Rules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONDITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file: EcmFileWorkflowConfiguration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ecmFile.fileType.equalsIgnoreCase("$param") || "$param".equals("*")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setStartProcess($param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setProcessName("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setTaskPriority($param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setTaskDueDateExpression("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setTaskName("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setApprovers("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setRequestType("$param");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$file.setBuckslipProcess($param);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If different rules apply to the same document, the last rule wins.  Be sure to put default rules first, and specific rules later.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start a Workflow Process? (true/false)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of business process to start (must be an Activiti process name)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority of user tasks (must be a number between 0 and 100; higher number is higher priority)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due date of user tasks.  Must be a valid ISO801 duration expression.  Examples: P3D = three days from now; P3H = 3 hours from now.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma-separated list of user ids; these users will be the reviewers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Business-meaningful process name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is buckslip process?               false is by default.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Workflow (no other rules match)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close Complaint Request</t>
-  </si>
-  <si>
-    <t xml:space="preserve">close_complaint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acmDocumentWorkflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Report of Investigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buckslip Complaint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complaint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ArkCaseBuckslipProcess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ann-acm@armedia.com,ian-acm@armedia.com,samuel-acm@armedia.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Case Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">change_case_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buckslip Case File</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review and Approve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Costsheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costsheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timesheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timesheet</t>
+    <t>Sequential</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>RuleTable Form Workflow Rules</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>$file: EcmFileWorkflowConfiguration</t>
+  </si>
+  <si>
+    <t>ecmFile.fileType.equalsIgnoreCase("$param") || "$param".equals("*")</t>
+  </si>
+  <si>
+    <t>$file.setStartProcess($param);</t>
+  </si>
+  <si>
+    <t>$file.setProcessName("$param");</t>
+  </si>
+  <si>
+    <t>$file.setTaskPriority($param);</t>
+  </si>
+  <si>
+    <t>$file.setTaskDueDateExpression("$param");</t>
+  </si>
+  <si>
+    <t>$file.setTaskName("$param");</t>
+  </si>
+  <si>
+    <t>$file.setApprovers("$param");</t>
+  </si>
+  <si>
+    <t>$file.setRequestType("$param");</t>
+  </si>
+  <si>
+    <t>$file.setBuckslipProcess($param);</t>
+  </si>
+  <si>
+    <t>If different rules apply to the same document, the last rule wins.  Be sure to put default rules first, and specific rules later.</t>
+  </si>
+  <si>
+    <t>Rule Name</t>
+  </si>
+  <si>
+    <t>File Type</t>
+  </si>
+  <si>
+    <t>Start a Workflow Process? (true/false)</t>
+  </si>
+  <si>
+    <t>Name of business process to start (must be an Activiti process name)</t>
+  </si>
+  <si>
+    <t>Priority of user tasks (must be a number between 0 and 100; higher number is higher priority)</t>
+  </si>
+  <si>
+    <t>Due date of user tasks.  Must be a valid ISO801 duration expression.  Examples: P3D = three days from now; P3H = 3 hours from now.</t>
+  </si>
+  <si>
+    <t>Task name</t>
+  </si>
+  <si>
+    <t>Comma-separated list of user ids; these users will be the reviewers.</t>
+  </si>
+  <si>
+    <t>Business-meaningful process name</t>
+  </si>
+  <si>
+    <t>is buckslip process?               false is by default.</t>
+  </si>
+  <si>
+    <t>Default Workflow (no other rules match)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Close Complaint Request</t>
+  </si>
+  <si>
+    <t>close_complaint</t>
+  </si>
+  <si>
+    <t>acmDocumentWorkflow</t>
+  </si>
+  <si>
+    <t>P3D</t>
+  </si>
+  <si>
+    <t>Report of Investigation</t>
+  </si>
+  <si>
+    <t>roi</t>
+  </si>
+  <si>
+    <t>Buckslip Complaint</t>
+  </si>
+  <si>
+    <t>complaint</t>
+  </si>
+  <si>
+    <t>ArkCaseBuckslipProcess</t>
+  </si>
+  <si>
+    <t>ann-acm@armedia.com,ian-acm@armedia.com,samuel-acm@armedia.com</t>
+  </si>
+  <si>
+    <t>Change Case Status</t>
+  </si>
+  <si>
+    <t>change_case_status</t>
+  </si>
+  <si>
+    <t>Buckslip Case File</t>
+  </si>
+  <si>
+    <t>case_file</t>
+  </si>
+  <si>
+    <t>Review and Approve</t>
+  </si>
+  <si>
+    <t>Costsheet</t>
+  </si>
+  <si>
+    <t>costsheet</t>
+  </si>
+  <si>
+    <t>Timesheet</t>
+  </si>
+  <si>
+    <t>timesheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -407,7 +395,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -466,230 +454,230 @@
     </fill>
   </fills>
   <borders count="12">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -748,13 +736,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -768,9 +772,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -782,7 +792,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -792,9 +802,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -813,9 +829,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -827,7 +849,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -837,9 +859,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -858,9 +886,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -872,7 +906,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -882,9 +916,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -903,9 +943,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -917,7 +963,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -927,9 +973,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -948,9 +1000,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -962,7 +1020,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -972,9 +1030,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -993,9 +1057,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1007,7 +1077,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1017,9 +1087,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1038,9 +1114,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1052,7 +1134,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1062,9 +1144,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1083,9 +1171,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="9" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1097,7 +1191,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1107,9 +1201,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1128,9 +1228,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="10" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1142,7 +1248,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1152,9 +1258,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1173,9 +1285,15 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="11" name="CustomShape 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1187,7 +1305,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -1197,46 +1315,836 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1044" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1042" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1040" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1038" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1036" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1034" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="65.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.71"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="65.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1245,7 +2153,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -1258,7 +2166,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -1271,7 +2179,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
@@ -1284,7 +2192,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="s">
@@ -1297,7 +2205,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5" t="s">
@@ -1310,7 +2218,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
@@ -1323,7 +2231,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7" t="s">
@@ -1336,7 +2244,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="255" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
@@ -1349,7 +2257,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10" t="s">
@@ -1362,7 +2270,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1371,7 +2279,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
@@ -1386,7 +2294,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="7" t="s">
@@ -1417,7 +2325,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="7" t="s">
@@ -1432,7 +2340,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="13" t="s">
@@ -1463,7 +2371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>26</v>
       </c>
@@ -1498,7 +2406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>37</v>
@@ -1517,7 +2425,7 @@
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="20" t="s">
         <v>40</v>
@@ -1531,7 +2439,7 @@
       <c r="E18" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="23" t="n">
+      <c r="F18" s="23">
         <v>50</v>
       </c>
       <c r="G18" s="23" t="s">
@@ -1542,7 +2450,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
         <v>44</v>
@@ -1556,7 +2464,7 @@
       <c r="E19" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="23" t="n">
+      <c r="F19" s="23">
         <v>50</v>
       </c>
       <c r="G19" s="23" t="s">
@@ -1567,7 +2475,7 @@
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="20" t="s">
         <v>46</v>
@@ -1581,13 +2489,15 @@
       <c r="E20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="23" t="n">
+      <c r="F20" s="23">
         <v>50</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="I20" s="23" t="s">
         <v>49</v>
       </c>
@@ -1596,7 +2506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>50</v>
@@ -1610,7 +2520,7 @@
       <c r="E21" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="23" t="n">
+      <c r="F21" s="23">
         <v>50</v>
       </c>
       <c r="G21" s="23" t="s">
@@ -1621,7 +2531,7 @@
       <c r="J21" s="23"/>
       <c r="K21" s="23"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="20" t="s">
         <v>52</v>
@@ -1635,7 +2545,7 @@
       <c r="E22" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="23" t="n">
+      <c r="F22" s="23">
         <v>50</v>
       </c>
       <c r="G22" s="23" t="s">
@@ -1652,7 +2562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
         <v>55</v>
@@ -1666,7 +2576,7 @@
       <c r="E23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="23" t="n">
+      <c r="F23" s="23">
         <v>50</v>
       </c>
       <c r="G23" s="23" t="s">
@@ -1677,7 +2587,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
         <v>57</v>
@@ -1691,7 +2601,7 @@
       <c r="E24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="23" t="n">
+      <c r="F24" s="23">
         <v>50</v>
       </c>
       <c r="G24" s="23" t="s">
@@ -1702,7 +2612,7 @@
       <c r="J24" s="23"/>
       <c r="K24" s="23"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="24"/>
@@ -1715,7 +2625,7 @@
       <c r="J25" s="23"/>
       <c r="K25" s="23"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
       <c r="C26" s="24"/>
@@ -1728,7 +2638,7 @@
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
       <c r="C27" s="24"/>
@@ -1741,7 +2651,7 @@
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="20"/>
       <c r="C28" s="24"/>
@@ -1756,70 +2666,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I22" r:id="rId2" display="ann-acm@armedia.com"/>
+    <hyperlink ref="I22" r:id="rId1" display="ann-acm@armedia.com"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.71"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.71"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AFDP-7754 - Need to create a new workflow for the new task created from a document
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.serafimoska\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.sanevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B50116-D860-4687-860E-0DBF671FAA32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0" shapeId="0">
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -91,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -121,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0" shapeId="0">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0" shapeId="0">
+    <comment ref="K16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -186,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
   <si>
     <t>RuleSet</t>
   </si>
@@ -371,15 +372,30 @@
   <si>
     <t>timesheet</t>
   </si>
+  <si>
+    <t>ArrestWarrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>arrestWarrant</t>
+  </si>
+  <si>
+    <t>Review Arrest Warrant</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -399,6 +415,14 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -621,10 +645,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -672,8 +697,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2118,14 +2147,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,16 +2643,34 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="B25" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="23">
+        <v>50</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
+      <c r="K25" s="23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
@@ -2666,17 +2713,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I22" r:id="rId1" display="ann-acm@armedia.com"/>
+    <hyperlink ref="I22" r:id="rId1" display="ann-acm@armedia.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I25" r:id="rId2" xr:uid="{C1AC9B01-C98D-4B2C-8EE4-2146AE10C06D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -2695,7 +2743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>

</xml_diff>

<commit_message>
removed timesheet and costsheet from this drools rule file
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrijana.maneva\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEA5FF0-62E1-4B80-B7E5-1C4A55CE15CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070387A7-F1D7-49BA-84F3-63F8307A66E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>RuleSet</t>
   </si>
@@ -356,18 +356,6 @@
   </si>
   <si>
     <t>Review and Approve</t>
-  </si>
-  <si>
-    <t>Costsheet</t>
-  </si>
-  <si>
-    <t>costsheet</t>
-  </si>
-  <si>
-    <t>Timesheet</t>
-  </si>
-  <si>
-    <t>timesheet</t>
   </si>
   <si>
     <t>ArrestWarrant</t>
@@ -1368,7 +1356,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1417,7 +1405,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1466,7 +1454,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1515,7 +1503,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1564,7 +1552,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1613,7 +1601,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1662,7 +1650,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1711,7 +1699,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1760,7 +1748,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1809,7 +1797,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2151,10 +2139,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,7 +2516,7 @@
         <v>53</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J20" s="23"/>
       <c r="K20" s="23" t="s">
@@ -2584,7 +2572,7 @@
         <v>53</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J22" s="23"/>
       <c r="K22" s="23" t="s">
@@ -2600,10 +2588,10 @@
         <v>55</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F23" s="23">
         <v>50</v>
@@ -2611,31 +2599,25 @@
       <c r="G23" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
+      <c r="H23" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>59</v>
+      </c>
       <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
+      <c r="K23" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="23">
-        <v>50</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>43</v>
-      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
@@ -2643,34 +2625,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="B25" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="23">
-        <v>50</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23" t="s">
-        <v>60</v>
-      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
@@ -2682,39 +2646,13 @@
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I25" r:id="rId2" xr:uid="{C1AC9B01-C98D-4B2C-8EE4-2146AE10C06D}"/>
+    <hyperlink ref="I23" r:id="rId2" xr:uid="{C1AC9B01-C98D-4B2C-8EE4-2146AE10C06D}"/>
     <hyperlink ref="I20" r:id="rId3" xr:uid="{AE8FE7C9-AA14-41E7-8956-26EE48AFF0AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-8562 removed costsheet and timesheet rule and changed change_case_status value to false
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrijana.maneva\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070387A7-F1D7-49BA-84F3-63F8307A66E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D6402E-6A02-4B2D-843E-000F6DBEF033}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -686,6 +686,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2142,7 +2145,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,7 +2534,7 @@
       <c r="C21" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="27" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="23" t="s">

</xml_diff>

<commit_message>
Replaced drools file with working one.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrijana.maneva\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\Desktop\Rules-To-Push\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D6402E-6A02-4B2D-843E-000F6DBEF033}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4089CA23-1569-4055-9537-B6FCDCFF5313}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
   <si>
     <t>RuleSet</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>ann-acm@armedia.com,ian-acm@armedia.com,samuel-acm@armedia.com</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>50</t>
   </si>
 </sst>
 </file>
@@ -2142,26 +2148,26 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="49.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
-    <col min="9" max="9" width="65.140625" customWidth="1"/>
-    <col min="10" max="10" width="30.28515625" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="65.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2437,13 +2443,27 @@
       <c r="D17" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="E17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
@@ -2459,16 +2479,24 @@
       <c r="E18" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="23">
-        <v>50</v>
+      <c r="F18" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
+      <c r="H18" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
@@ -2484,16 +2512,24 @@
       <c r="E19" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="23">
-        <v>50</v>
+      <c r="F19" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="G19" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="H19" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
@@ -2509,8 +2545,8 @@
       <c r="E20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="23">
-        <v>50</v>
+      <c r="F20" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>43</v>
@@ -2521,7 +2557,9 @@
       <c r="I20" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="J20" s="23"/>
+      <c r="J20" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="K20" s="23" t="s">
         <v>12</v>
       </c>
@@ -2540,16 +2578,24 @@
       <c r="E21" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="23">
-        <v>50</v>
+      <c r="F21" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="G21" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
+      <c r="H21" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
@@ -2565,8 +2611,8 @@
       <c r="E22" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="23">
-        <v>50</v>
+      <c r="F22" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>43</v>
@@ -2577,7 +2623,9 @@
       <c r="I22" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="K22" s="23" t="s">
         <v>12</v>
       </c>
@@ -2596,8 +2644,8 @@
       <c r="E23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="23">
-        <v>50</v>
+      <c r="F23" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>43</v>
@@ -2608,47 +2656,101 @@
       <c r="I23" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="J23" s="23"/>
+      <c r="J23" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="K23" s="23" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
+      <c r="B24" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="B25" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="B26" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
     </row>
@@ -2670,13 +2772,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AMK1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2689,13 +2791,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AMK1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-8721 Change the specified users in buckslip approval workflows to arkcase.org domains
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasko.tanaskoski\Desktop\Rules-To-Push\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksandar.acevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4089CA23-1569-4055-9537-B6FCDCFF5313}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6CCCFD-A89A-4D85-8F23-92D2C27F411D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
   <si>
     <t>RuleSet</t>
   </si>
@@ -373,13 +373,13 @@
     <t>Review Arrest Warrant</t>
   </si>
   <si>
-    <t>ann-acm@armedia.com,ian-acm@armedia.com,samuel-acm@armedia.com</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>50</t>
+  </si>
+  <si>
+    <t>ann-acm@arkcase.org,sally-acm@arkcase.org,samuel-acm@arkcase.org</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -853,7 +853,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -910,7 +910,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -967,7 +967,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1024,7 +1024,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1081,7 +1081,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1138,7 +1138,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1195,7 +1195,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1252,7 +1252,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1309,7 +1309,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>180915</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2150,27 +2150,27 @@
   </sheetPr>
   <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="65.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.86328125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.73046875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.73046875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.1328125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35.59765625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.73046875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="65.1328125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.265625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.73046875" customWidth="1" collapsed="1"/>
+    <col min="12" max="1025" width="8.73046875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2179,7 +2179,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -2192,7 +2192,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -2205,7 +2205,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
@@ -2218,7 +2218,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="s">
@@ -2231,7 +2231,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5" t="s">
@@ -2244,7 +2244,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
@@ -2257,7 +2257,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7" t="s">
@@ -2270,7 +2270,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="213.75" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
@@ -2283,7 +2283,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10" t="s">
@@ -2296,7 +2296,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2305,7 +2305,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
@@ -2320,7 +2320,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="7" t="s">
@@ -2351,7 +2351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="7" t="s">
@@ -2366,7 +2366,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="13" t="s">
@@ -2397,7 +2397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>26</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>37</v>
@@ -2444,28 +2444,28 @@
         <v>39</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="19"/>
       <c r="B18" s="20" t="s">
         <v>40</v>
@@ -2480,25 +2480,25 @@
         <v>42</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>43</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
         <v>44</v>
@@ -2513,25 +2513,25 @@
         <v>42</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" s="23" t="s">
         <v>43</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="19"/>
       <c r="B20" s="20" t="s">
         <v>46</v>
@@ -2546,7 +2546,7 @@
         <v>48</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>43</v>
@@ -2555,16 +2555,16 @@
         <v>53</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>49</v>
@@ -2579,25 +2579,25 @@
         <v>42</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G21" s="23" t="s">
         <v>43</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K21" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="19"/>
       <c r="B22" s="20" t="s">
         <v>51</v>
@@ -2612,7 +2612,7 @@
         <v>48</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>43</v>
@@ -2621,16 +2621,16 @@
         <v>53</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K22" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
         <v>54</v>
@@ -2645,7 +2645,7 @@
         <v>57</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>43</v>
@@ -2654,116 +2654,116 @@
         <v>58</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
       <c r="B25" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="19"/>
       <c r="B26" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I23" r:id="rId2" xr:uid="{C1AC9B01-C98D-4B2C-8EE4-2146AE10C06D}"/>
-    <hyperlink ref="I20" r:id="rId3" xr:uid="{AE8FE7C9-AA14-41E7-8956-26EE48AFF0AC}"/>
+    <hyperlink ref="I23" r:id="rId1" xr:uid="{9CAAFBA4-288C-46BC-86F9-3FB1B05525DD}"/>
+    <hyperlink ref="I22" r:id="rId2" xr:uid="{99F591C3-4BE3-4FEA-BA65-85D8D4FE2478}"/>
+    <hyperlink ref="I20" r:id="rId3" xr:uid="{98B6CF15-E635-44A2-A694-26546654BB20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2776,9 +2776,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1025" width="8.73046875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2795,9 +2795,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1025" width="8.73046875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-8961 Add consultation status change to form business process rules
</commit_message>
<xml_diff>
--- a/acm/rules/drools-form-business-process-rules.xlsx
+++ b/acm/rules/drools-form-business-process-rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksandar.acevski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6CCCFD-A89A-4D85-8F23-92D2C27F411D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C62963-0D67-4635-ADBE-A0A541765789}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>RuleSet</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>ann-acm@arkcase.org,sally-acm@arkcase.org,samuel-acm@arkcase.org</t>
+  </si>
+  <si>
+    <t>Change Consultation Status</t>
   </si>
 </sst>
 </file>
@@ -795,8 +798,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -852,8 +855,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -909,8 +912,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -966,8 +969,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1023,8 +1026,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1080,8 +1083,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1137,8 +1140,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1194,8 +1197,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1251,8 +1254,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1308,8 +1311,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1028880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180915</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>371415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2150,27 +2153,27 @@
   </sheetPr>
   <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.265625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="49.86328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.73046875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.73046875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.1328125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35.59765625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.73046875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="65.1328125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.265625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.73046875" customWidth="1" collapsed="1"/>
-    <col min="12" max="1025" width="8.73046875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="65.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2179,7 +2182,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -2192,7 +2195,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -2205,7 +2208,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
@@ -2218,7 +2221,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="s">
@@ -2231,7 +2234,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="5" t="s">
@@ -2244,7 +2247,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
@@ -2257,7 +2260,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7" t="s">
@@ -2270,7 +2273,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
@@ -2283,7 +2286,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10" t="s">
@@ -2296,7 +2299,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2305,7 +2308,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
@@ -2320,7 +2323,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="7" t="s">
@@ -2351,7 +2354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="7" t="s">
@@ -2366,7 +2369,7 @@
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="13" t="s">
@@ -2397,7 +2400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>26</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>37</v>
@@ -2465,7 +2468,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="20" t="s">
         <v>40</v>
@@ -2498,7 +2501,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
         <v>44</v>
@@ -2531,7 +2534,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="20" t="s">
         <v>46</v>
@@ -2564,7 +2567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>49</v>
@@ -2597,7 +2600,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="20" t="s">
         <v>51</v>
@@ -2630,7 +2633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
         <v>54</v>
@@ -2663,25 +2666,25 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>59</v>
+        <v>50</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>56</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H24" s="23" t="s">
         <v>59</v>
@@ -2696,7 +2699,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="20" t="s">
         <v>59</v>
@@ -2725,7 +2728,7 @@
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="20" t="s">
         <v>59</v>
@@ -2776,9 +2779,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2795,9 +2798,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>